<commit_message>
Update : Update excel file
</commit_message>
<xml_diff>
--- a/Projet-Groupe1-DKM/data/trey_power_network.xlsx
+++ b/Projet-Groupe1-DKM/data/trey_power_network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eistore2\iese\institut\Laboratoires\Labo_MRB\RHT\Labo\teams_lab_pack_2024-2025\mini-projet-trey\input-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\root\git\rhtlab_DKM\Projet-Groupe1-DKM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD5684B-AA1E-4BE0-9588-B2D026B68503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447352A7-6166-41C0-8927-E6F476010644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -443,10 +443,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Insatisfaisant" xfId="3" builtinId="27"/>
+    <cellStyle name="Neutre" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -462,7 +462,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -760,17 +760,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD154A9-14F2-4509-A0AA-B0D37BD7BC37}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -790,7 +790,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -804,7 +804,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -818,7 +818,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -832,7 +832,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -846,7 +846,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -860,7 +860,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -874,7 +874,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -888,7 +888,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -902,7 +902,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -916,7 +916,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -930,7 +930,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -944,7 +944,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -958,13 +958,16 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>97</v>
       </c>
+      <c r="C14">
+        <v>18.3</v>
+      </c>
       <c r="D14" t="s">
         <v>69</v>
       </c>
@@ -972,92 +975,92 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1076,18 +1079,18 @@
       <selection activeCell="E2" sqref="E2:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" customWidth="1"/>
-    <col min="11" max="11" width="10.36328125" customWidth="1"/>
-    <col min="12" max="12" width="15.6328125" customWidth="1"/>
-    <col min="13" max="13" width="16.36328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1171,7 +1174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1186,7 +1189,7 @@
       </c>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1201,7 +1204,7 @@
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1215,7 +1218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1244,7 +1247,7 @@
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1259,7 +1262,7 @@
       </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1287,7 +1290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1301,102 +1304,102 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1414,12 +1417,12 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1451,157 +1454,157 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1619,17 +1622,17 @@
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="15" max="15" width="14.08984375" customWidth="1"/>
-    <col min="17" max="17" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.453125" customWidth="1"/>
-    <col min="24" max="24" width="19.453125" customWidth="1"/>
-    <col min="26" max="26" width="18.6328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.44140625" customWidth="1"/>
+    <col min="24" max="24" width="19.44140625" customWidth="1"/>
+    <col min="26" max="26" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -1721,7 +1724,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1756,152 +1759,152 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1919,15 +1922,15 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" style="8"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="8"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1989,153 +1992,153 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2154,17 +2157,17 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="2" max="7" width="10.6328125" customWidth="1"/>
-    <col min="8" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="10.6328125" customWidth="1"/>
-    <col min="12" max="12" width="17.08984375" customWidth="1"/>
-    <col min="13" max="24" width="10.6328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" customWidth="1"/>
+    <col min="13" max="24" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2205,157 +2208,157 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2371,19 +2374,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB91AA0C-6E10-4C2C-B831-A2E20673E5F8}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="7" max="7" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2421,7 +2424,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2432,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2443,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2454,7 +2457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2465,7 +2468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2476,7 +2479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2487,7 +2490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2498,7 +2501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2509,7 +2512,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2531,7 +2534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2553,97 +2556,97 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Puissance active et réactive pour faire un test de fonctionnment
</commit_message>
<xml_diff>
--- a/Projet-Groupe1-DKM/data/trey_power_network.xlsx
+++ b/Projet-Groupe1-DKM/data/trey_power_network.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\root\git\rhtlab_DKM\Projet-Groupe1-DKM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\karim\git\rhtlab_DKM\Projet-Groupe1-DKM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062BFA65-CC3A-47BF-9058-CE2CDAE48CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4293AEAB-DD16-43A9-B3E0-0F965CAEF81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -2584,7 +2584,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2643,6 +2643,12 @@
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="D2">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -2654,6 +2660,12 @@
       <c r="C3">
         <v>1</v>
       </c>
+      <c r="D3">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E3">
+        <v>1.35E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -2665,6 +2677,12 @@
       <c r="C4">
         <v>2</v>
       </c>
+      <c r="D4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E4">
+        <v>3.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -2676,6 +2694,12 @@
       <c r="C5">
         <v>3</v>
       </c>
+      <c r="D5">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E5">
+        <v>4.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -2687,6 +2711,12 @@
       <c r="C6">
         <v>4</v>
       </c>
+      <c r="D6">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E6">
+        <v>4.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -2698,6 +2728,12 @@
       <c r="C7">
         <v>5</v>
       </c>
+      <c r="D7">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E7">
+        <v>3.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -2709,6 +2745,12 @@
       <c r="C8">
         <v>6</v>
       </c>
+      <c r="D8">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>1.0500000000000001E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -2720,6 +2762,12 @@
       <c r="C9">
         <v>7</v>
       </c>
+      <c r="D9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E9">
+        <v>5.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -2731,6 +2779,12 @@
       <c r="C10">
         <v>8</v>
       </c>
+      <c r="D10">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E10">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -2742,6 +2796,12 @@
       <c r="C11">
         <v>9</v>
       </c>
+      <c r="D11">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E11">
+        <v>4.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -2753,6 +2813,12 @@
       <c r="C12">
         <v>10</v>
       </c>
+      <c r="D12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E12">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -2763,6 +2829,12 @@
       </c>
       <c r="C13">
         <v>11</v>
+      </c>
+      <c r="D13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E13">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update scaling load excel
</commit_message>
<xml_diff>
--- a/Projet-Groupe1-DKM/data/trey_power_network.xlsx
+++ b/Projet-Groupe1-DKM/data/trey_power_network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\karim\git\rhtlab_DKM\Projet-Groupe1-DKM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4293AEAB-DD16-43A9-B3E0-0F965CAEF81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74414D0F-0AC7-46B4-B5C7-FC416CE17601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -2584,7 +2584,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2649,6 +2649,9 @@
       <c r="E2">
         <v>0.01</v>
       </c>
+      <c r="F2">
+        <v>456464</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">

</xml_diff>

<commit_message>
avancement de la simulation
</commit_message>
<xml_diff>
--- a/Projet-Groupe1-DKM/data/trey_power_network.xlsx
+++ b/Projet-Groupe1-DKM/data/trey_power_network.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\karim\git\rhtlab_DKM\Projet-Groupe1-DKM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC28103C-64E9-440A-8211-4435DE4EAD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2744B7D7-3B5A-49A0-B101-6F7CE36AE3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
@@ -2363,7 +2363,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2427,6 +2427,9 @@
       <c r="C2">
         <v>10</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="H2">
         <v>0</v>
       </c>
@@ -2440,6 +2443,9 @@
       </c>
       <c r="C3">
         <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>

</xml_diff>

<commit_message>
Création du plot pour les charges sur la lignes
</commit_message>
<xml_diff>
--- a/Projet-Groupe1-DKM/data/trey_power_network.xlsx
+++ b/Projet-Groupe1-DKM/data/trey_power_network.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\karim\git\rhtlab_DKM\Projet-Groupe1-DKM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2744B7D7-3B5A-49A0-B101-6F7CE36AE3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13804AC-9CBB-498C-9A26-510F41CA55BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
@@ -2363,7 +2363,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2428,7 +2428,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -2445,7 +2445,7 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>1</v>

</xml_diff>

<commit_message>
Correction d'un facteur de 100 sur le courant admissible sur la ligne
</commit_message>
<xml_diff>
--- a/Projet-Groupe1-DKM/data/trey_power_network.xlsx
+++ b/Projet-Groupe1-DKM/data/trey_power_network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\karim\git\rhtlab_DKM\Projet-Groupe1-DKM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13804AC-9CBB-498C-9A26-510F41CA55BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BF558E-ECF7-478C-AC6A-D55B4574FBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -1114,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D466C24-507B-41DF-96AE-5E0A3D434556}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1211,7 +1211,7 @@
         <v>0.34899999999999998</v>
       </c>
       <c r="I2">
-        <v>400</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -1240,7 +1240,7 @@
         <v>0.34899999999999998</v>
       </c>
       <c r="I3">
-        <v>400</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -1269,7 +1269,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="I4">
-        <v>252</v>
+        <v>0.252</v>
       </c>
       <c r="K4" s="5"/>
     </row>
@@ -1299,7 +1299,7 @@
         <v>0.29799999999999999</v>
       </c>
       <c r="I5">
-        <v>170</v>
+        <v>0.17</v>
       </c>
       <c r="K5" s="5"/>
     </row>
@@ -1329,7 +1329,7 @@
         <v>0.29799999999999999</v>
       </c>
       <c r="I6">
-        <v>170</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -1358,7 +1358,7 @@
         <v>0.34899999999999998</v>
       </c>
       <c r="I7">
-        <v>400</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -1387,7 +1387,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="I8">
-        <v>252</v>
+        <v>0.252</v>
       </c>
       <c r="K8" s="5"/>
     </row>
@@ -1417,7 +1417,7 @@
         <v>0.34899999999999998</v>
       </c>
       <c r="I9">
-        <v>400</v>
+        <v>0.4</v>
       </c>
       <c r="K9" s="5"/>
     </row>
@@ -1447,7 +1447,7 @@
         <v>0.29799999999999999</v>
       </c>
       <c r="I10">
-        <v>170</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -1476,7 +1476,7 @@
         <v>0.29799999999999999</v>
       </c>
       <c r="I11">
-        <v>170</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -1505,7 +1505,7 @@
         <v>0.34599999999999997</v>
       </c>
       <c r="I12">
-        <v>512</v>
+        <v>0.51200000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -2362,7 +2362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0724F9-1790-4ECA-B4EA-D773CFA5B42B}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>